<commit_message>
Library corrections and additions
changed o-tatum-format to u-tatum-format; o-list-trans revised; created
u-list-duplicator object and implemented it in the library overview and
helpfiles.
</commit_message>
<xml_diff>
--- a/Tessellate Objects List.xlsx
+++ b/Tessellate Objects List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="7040" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="3040" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>TESSELLATE OBJECTS</t>
   </si>
@@ -30,27 +30,18 @@
     <t>Count elements in a list and truncate to number of elements specified</t>
   </si>
   <si>
-    <t>O-CRIBS</t>
-  </si>
-  <si>
     <t>O-EQUAL-PROBABILITY</t>
   </si>
   <si>
     <t>crib the list or list of lists.</t>
   </si>
   <si>
-    <t>A rhythm crib builder--crib the list or list of lists.</t>
-  </si>
-  <si>
     <t>O-INDEX</t>
   </si>
   <si>
     <t>GET INDEX (default): multiple source lists w/ multiple index list; GET INDEX (optional mode=1): single source list, multiple index lists</t>
   </si>
   <si>
-    <t>O-LIST-INFO</t>
-  </si>
-  <si>
     <t>Returns the length and sum of all sublists separately and returns the result retaining the original list structure. The output takes the form:((no. of elements, sum) (no. of elements, sum) ...etc)) for each list of lists provided. The last element of each sublist is the total sum of the sublist elements. Default ("rhythm-lists" takes a nested list of lists. Mode 1 ("pitches") mode takes in a simple lists of lists. Mode 2 ("tatums") mode takes in a list of tatum lists.</t>
   </si>
   <si>
@@ -69,21 +60,12 @@
     <t>O-LIST-TRANS</t>
   </si>
   <si>
-    <t>Returns a list of random elements from listA or listB following a bpf to guide the probability from which list (A or B) a given element is chosen.</t>
-  </si>
-  <si>
     <t>O-SUM-LISTS</t>
   </si>
   <si>
     <t>Sums all sublists and returns the result.</t>
   </si>
   <si>
-    <t>O-TATUM-FORMAT</t>
-  </si>
-  <si>
-    <t>O-tatum-format converts a tatum shorthand into a notation suitable for use with tessellate score objects.  Second output provides sum of total elements.</t>
-  </si>
-  <si>
     <t>P-BANDS-COLLECTION</t>
   </si>
   <si>
@@ -346,6 +328,18 @@
   </si>
   <si>
     <t>U-SCORE-LISTS</t>
+  </si>
+  <si>
+    <t>U-LIST-INFO</t>
+  </si>
+  <si>
+    <t>U-TATUM-FORMAT</t>
+  </si>
+  <si>
+    <t>Converts a tatum shorthand into a notation suitable for use with tessellate score objects.  Second output provides sum of total elements.</t>
+  </si>
+  <si>
+    <t>Returns a list of random elements from listA or listB following a bpf to guide the probability from which list (A or B) a given element is chosen. Allows for weighted probabilities.</t>
   </si>
 </sst>
 </file>
@@ -358,7 +352,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -406,8 +400,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -421,15 +419,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -759,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:C59"/>
+  <dimension ref="B4:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,20 +791,20 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -818,18 +820,18 @@
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -901,12 +903,12 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -925,12 +927,12 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>40</v>
@@ -994,127 +996,127 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
         <v>55</v>
-      </c>
-      <c r="C33" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="B40" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="2:3">
       <c r="B43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="2:3">
       <c r="B46" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="2:3">
       <c r="B48" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
         <v>71</v>
@@ -1122,90 +1124,82 @@
     </row>
     <row r="49" spans="2:3">
       <c r="B49" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="2:3">
       <c r="B51" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="2:3">
       <c r="B52" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="2:3">
       <c r="B55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="B58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3">
-      <c r="B59" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>